<commit_message>
Update rs according to comments
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
@@ -11581,9 +11581,6 @@
     <t>[In Prerequisites/Preconditions] The mechanism for obtaining these credentials [the credentials of the client] is specific to the protocol of the security provider that is used.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation does not modify any properties of any objects in the address book. (Exchange 2010SP3 and below follow this behavior).</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does follow the ABNF format. (Microsoft Exchange Server 2010 Service Pack 3 (SP3) follows this behavior).</t>
   </si>
   <si>
@@ -11597,6 +11594,9 @@
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Implementation does not ignore this request [a value of "fAnonymousLogin" in the input parameter dwFlags]. (Exchange 2010 and above follow this behavior.)</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does not modify any properties of any objects in the address book. (Microsoft Exchange Server 2010 Service Pack 3 (SP3) follows this behavior).</t>
   </si>
 </sst>
 </file>
@@ -11880,21 +11880,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11918,6 +11903,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13342,8 +13342,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1511" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1518" sqref="C1518"/>
+    <sheetView tabSelected="1" topLeftCell="A1519" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1526" sqref="C1526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -13398,127 +13398,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -13531,12 +13531,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -13549,12 +13549,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -13567,12 +13567,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -13585,60 +13585,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -33701,7 +33701,7 @@
         <v>17</v>
       </c>
       <c r="I809" s="20" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="810" spans="1:9" ht="60">
@@ -41558,7 +41558,7 @@
         <v>17</v>
       </c>
       <c r="I1120" s="20" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="1121" spans="1:9" ht="60">
@@ -51639,7 +51639,7 @@
         <v>3171</v>
       </c>
       <c r="C1517" s="20" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="D1517" s="22" t="s">
         <v>3181</v>
@@ -51666,7 +51666,7 @@
         <v>3171</v>
       </c>
       <c r="C1518" s="20" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="D1518" s="22" t="s">
         <v>3183</v>
@@ -51778,7 +51778,7 @@
         <v>7</v>
       </c>
       <c r="C1522" s="33" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="D1522" s="22" t="s">
         <v>3617</v>
@@ -51894,7 +51894,7 @@
         <v>7</v>
       </c>
       <c r="C1526" s="33" t="s">
-        <v>3640</v>
+        <v>3645</v>
       </c>
       <c r="D1526" s="22" t="s">
         <v>3619</v>
@@ -54692,6 +54692,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -54699,11 +54704,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1542:B1545 A1548:B1549 A1637:I1637 A1634:H1634 D1542:I1545 A1546:I1547 A1550:I1566 D1548:I1549 A1600:I1633 A20:I46 A1570:I1597 E1567:H1569 D1598:H1599 D1635:H1636 G47:G48 I47:K48 A49:I1541">

</xml_diff>

<commit_message>
update R52 R53 R53001
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -11602,7 +11602,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -11880,21 +11880,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11918,6 +11903,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13095,7 +13095,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13130,7 +13130,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13342,7 +13342,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1641"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H138" sqref="H138"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -13396,127 +13398,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -13529,12 +13531,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -13547,12 +13549,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -13565,12 +13567,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -13583,60 +13585,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -16548,13 +16550,13 @@
         <v>19</v>
       </c>
       <c r="F133" s="22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G133" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H133" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I133" s="20"/>
     </row>
@@ -16573,13 +16575,13 @@
         <v>19</v>
       </c>
       <c r="F134" s="22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G134" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H134" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I134" s="20"/>
     </row>
@@ -16604,7 +16606,7 @@
         <v>15</v>
       </c>
       <c r="H135" s="32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I135" s="34"/>
     </row>
@@ -54690,6 +54692,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -54697,11 +54704,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1542:B1545 A1548:B1549 A1637:I1637 A1634:H1634 D1542:I1545 A1546:I1547 A1550:I1566 D1548:I1549 A1600:I1633 A20:I46 A1570:I1597 E1567:H1569 D1598:H1599 D1635:H1636 G47:G48 I47:K48 A49:I1541">

</xml_diff>

<commit_message>
[MS-OXNSPI]: Update requirement for the new tdi 98670
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
@@ -11880,6 +11880,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11904,26 +11919,373 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="131">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -12516,368 +12878,6 @@
         <strike/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -13005,34 +13005,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1636" tableType="xml" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1636" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A19:I1636"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="128" dataCellStyle="Normal">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="127" dataCellStyle="Normal">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="126" dataCellStyle="Normal">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="125" dataCellStyle="Normal">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="124" dataCellStyle="Normal">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="123" dataCellStyle="Normal">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="122" dataCellStyle="Normal">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="121" dataCellStyle="Normal">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="120">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -13041,12 +13041,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="114"/>
-    <tableColumn id="2" name="Test" dataDxfId="113"/>
-    <tableColumn id="3" name="Description" dataDxfId="112"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13396,127 +13396,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -13529,12 +13529,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -13547,12 +13547,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -13565,12 +13565,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -13583,60 +13583,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -19642,7 +19642,7 @@
         <v>15</v>
       </c>
       <c r="H255" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I255" s="20"/>
     </row>
@@ -19667,7 +19667,7 @@
         <v>15</v>
       </c>
       <c r="H256" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I256" s="20"/>
     </row>
@@ -19692,7 +19692,7 @@
         <v>15</v>
       </c>
       <c r="H257" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I257" s="20"/>
     </row>
@@ -19716,8 +19716,8 @@
       <c r="G258" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H258" s="32" t="s">
-        <v>20</v>
+      <c r="H258" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="I258" s="34"/>
     </row>
@@ -54690,11 +54690,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -54702,421 +54697,426 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1542:B1545 A1548:B1549 A1637:I1637 A1634:H1634 D1542:I1545 A1546:I1547 A1550:I1566 D1548:I1549 A1600:I1633 A20:I46 A1570:I1597 E1567:H1569 D1598:H1599 D1635:H1636 G47:G48 I47:K48 A49:I1541">
-    <cfRule type="expression" dxfId="111" priority="192">
+    <cfRule type="expression" dxfId="130" priority="192">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="193">
+    <cfRule type="expression" dxfId="129" priority="193">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="194">
+    <cfRule type="expression" dxfId="128" priority="194">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1542:B1545 A1548:B1549 A1637:I1637 A1634:H1634 D1542:I1545 A1546:I1547 A1550:I1566 D1548:I1549 A1600:I1633 A20:I46 A1570:I1597 E1567:H1569 D1598:H1599 D1635:H1636 G47:G48 I47:K48 A49:I1541">
-    <cfRule type="expression" dxfId="108" priority="187">
+    <cfRule type="expression" dxfId="127" priority="187">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="188">
+    <cfRule type="expression" dxfId="126" priority="188">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="189">
+    <cfRule type="expression" dxfId="125" priority="189">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1637 F1536:F1537 F1540:F1566 F1600:F1634 F20:F46 F1570:F1597 F49:F1526">
-    <cfRule type="expression" dxfId="105" priority="190">
+    <cfRule type="expression" dxfId="124" priority="190">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="191">
+    <cfRule type="expression" dxfId="123" priority="191">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1567:I1569 I1598:I1599 I1634:I1636">
-    <cfRule type="expression" dxfId="103" priority="179">
+    <cfRule type="expression" dxfId="122" priority="179">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="180">
+    <cfRule type="expression" dxfId="121" priority="180">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="181">
+    <cfRule type="expression" dxfId="120" priority="181">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1567:I1569 I1598:I1599 I1634:I1636">
-    <cfRule type="expression" dxfId="100" priority="184">
+    <cfRule type="expression" dxfId="119" priority="184">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="185">
+    <cfRule type="expression" dxfId="118" priority="185">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="186">
+    <cfRule type="expression" dxfId="117" priority="186">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1527:F1535">
-    <cfRule type="expression" dxfId="97" priority="182">
+    <cfRule type="expression" dxfId="116" priority="182">
       <formula>NOT(VLOOKUP(F1527,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="183">
+    <cfRule type="expression" dxfId="115" priority="183">
       <formula>(VLOOKUP(F1527,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1567:D1569">
-    <cfRule type="expression" dxfId="95" priority="159">
+    <cfRule type="expression" dxfId="114" priority="159">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="160">
+    <cfRule type="expression" dxfId="113" priority="160">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="161">
+    <cfRule type="expression" dxfId="112" priority="161">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1567:D1569">
-    <cfRule type="expression" dxfId="92" priority="162">
+    <cfRule type="expression" dxfId="111" priority="162">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="163">
+    <cfRule type="expression" dxfId="110" priority="163">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="164">
+    <cfRule type="expression" dxfId="109" priority="164">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1567:F1569">
-    <cfRule type="expression" dxfId="89" priority="154">
+    <cfRule type="expression" dxfId="108" priority="154">
       <formula>NOT(VLOOKUP(F1567,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="155">
+    <cfRule type="expression" dxfId="107" priority="155">
       <formula>(VLOOKUP(F1567,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1598:F1599">
-    <cfRule type="expression" dxfId="87" priority="146">
+    <cfRule type="expression" dxfId="106" priority="146">
       <formula>NOT(VLOOKUP(F1598,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="147">
+    <cfRule type="expression" dxfId="105" priority="147">
       <formula>(VLOOKUP(F1598,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1598:C1599">
-    <cfRule type="expression" dxfId="85" priority="137">
+    <cfRule type="expression" dxfId="104" priority="137">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="138">
+    <cfRule type="expression" dxfId="103" priority="138">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="139">
+    <cfRule type="expression" dxfId="102" priority="139">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1598:C1599">
-    <cfRule type="expression" dxfId="82" priority="140">
+    <cfRule type="expression" dxfId="101" priority="140">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="141">
+    <cfRule type="expression" dxfId="100" priority="141">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="142">
+    <cfRule type="expression" dxfId="99" priority="142">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1635:F1636">
-    <cfRule type="expression" dxfId="79" priority="132">
+    <cfRule type="expression" dxfId="98" priority="132">
       <formula>NOT(VLOOKUP(F1635,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="133">
+    <cfRule type="expression" dxfId="97" priority="133">
       <formula>(VLOOKUP(F1635,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1635:B1636">
-    <cfRule type="expression" dxfId="77" priority="120">
+    <cfRule type="expression" dxfId="96" priority="120">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="121">
+    <cfRule type="expression" dxfId="95" priority="121">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="122">
+    <cfRule type="expression" dxfId="94" priority="122">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1635:B1636">
-    <cfRule type="expression" dxfId="74" priority="117">
+    <cfRule type="expression" dxfId="93" priority="117">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="118">
+    <cfRule type="expression" dxfId="92" priority="118">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="119">
+    <cfRule type="expression" dxfId="91" priority="119">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1635:A1636 C1635:C1636">
-    <cfRule type="expression" dxfId="71" priority="123">
+    <cfRule type="expression" dxfId="90" priority="123">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="124">
+    <cfRule type="expression" dxfId="89" priority="124">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="125">
+    <cfRule type="expression" dxfId="88" priority="125">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1635:A1636 C1635:C1636">
-    <cfRule type="expression" dxfId="68" priority="126">
+    <cfRule type="expression" dxfId="87" priority="126">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="127">
+    <cfRule type="expression" dxfId="86" priority="127">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="128">
+    <cfRule type="expression" dxfId="85" priority="128">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1538:F1539">
-    <cfRule type="expression" dxfId="65" priority="100">
+    <cfRule type="expression" dxfId="84" priority="100">
       <formula>NOT(VLOOKUP(F1538,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="101">
+    <cfRule type="expression" dxfId="83" priority="101">
       <formula>(VLOOKUP(F1538,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1542:C1543">
-    <cfRule type="expression" dxfId="63" priority="88">
+    <cfRule type="expression" dxfId="82" priority="88">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="89">
+    <cfRule type="expression" dxfId="81" priority="89">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="90">
+    <cfRule type="expression" dxfId="80" priority="90">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1542:C1543">
-    <cfRule type="expression" dxfId="60" priority="85">
+    <cfRule type="expression" dxfId="79" priority="85">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="86">
+    <cfRule type="expression" dxfId="78" priority="86">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="87">
+    <cfRule type="expression" dxfId="77" priority="87">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1544:C1545">
-    <cfRule type="expression" dxfId="57" priority="76">
+    <cfRule type="expression" dxfId="76" priority="76">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="77">
+    <cfRule type="expression" dxfId="75" priority="77">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="78">
+    <cfRule type="expression" dxfId="74" priority="78">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1544:C1545">
-    <cfRule type="expression" dxfId="54" priority="73">
+    <cfRule type="expression" dxfId="73" priority="73">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="74">
+    <cfRule type="expression" dxfId="72" priority="74">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="75">
+    <cfRule type="expression" dxfId="71" priority="75">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1548:C1549">
-    <cfRule type="expression" dxfId="51" priority="64">
+    <cfRule type="expression" dxfId="70" priority="64">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="65">
+    <cfRule type="expression" dxfId="69" priority="65">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="66">
+    <cfRule type="expression" dxfId="68" priority="66">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1548:C1549">
-    <cfRule type="expression" dxfId="48" priority="61">
+    <cfRule type="expression" dxfId="67" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="62">
+    <cfRule type="expression" dxfId="66" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="63">
+    <cfRule type="expression" dxfId="65" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:E48">
-    <cfRule type="expression" dxfId="45" priority="58">
+    <cfRule type="expression" dxfId="64" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="59">
+    <cfRule type="expression" dxfId="63" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="60">
+    <cfRule type="expression" dxfId="62" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:E48">
-    <cfRule type="expression" dxfId="42" priority="53">
+    <cfRule type="expression" dxfId="61" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="54">
+    <cfRule type="expression" dxfId="60" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="55">
+    <cfRule type="expression" dxfId="59" priority="55">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:A48">
-    <cfRule type="expression" dxfId="39" priority="50">
+    <cfRule type="expression" dxfId="58" priority="50">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="51">
+    <cfRule type="expression" dxfId="57" priority="51">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="52">
+    <cfRule type="expression" dxfId="56" priority="52">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:A48">
-    <cfRule type="expression" dxfId="36" priority="47">
+    <cfRule type="expression" dxfId="55" priority="47">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="48">
+    <cfRule type="expression" dxfId="54" priority="48">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="49">
+    <cfRule type="expression" dxfId="53" priority="49">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="33" priority="44">
+    <cfRule type="expression" dxfId="52" priority="44">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="45">
+    <cfRule type="expression" dxfId="51" priority="45">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="46">
+    <cfRule type="expression" dxfId="50" priority="46">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="30" priority="41">
+    <cfRule type="expression" dxfId="49" priority="41">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="42">
+    <cfRule type="expression" dxfId="48" priority="42">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="43">
+    <cfRule type="expression" dxfId="47" priority="43">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="27" priority="38">
+    <cfRule type="expression" dxfId="46" priority="38">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="39">
+    <cfRule type="expression" dxfId="45" priority="39">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="40">
+    <cfRule type="expression" dxfId="44" priority="40">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="24" priority="35">
+    <cfRule type="expression" dxfId="43" priority="35">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="36">
+    <cfRule type="expression" dxfId="42" priority="36">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="37">
+    <cfRule type="expression" dxfId="41" priority="37">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="40" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="39" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="38" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="37" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="36" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="35" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="15" priority="20">
+    <cfRule type="expression" dxfId="34" priority="20">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="21">
+    <cfRule type="expression" dxfId="33" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="22">
+    <cfRule type="expression" dxfId="32" priority="22">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="31" priority="15">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="16">
+    <cfRule type="expression" dxfId="30" priority="16">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="17">
+    <cfRule type="expression" dxfId="29" priority="17">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="expression" dxfId="9" priority="18">
+    <cfRule type="expression" dxfId="28" priority="18">
       <formula>NOT(VLOOKUP(F47,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="27" priority="19">
       <formula>(VLOOKUP(F47,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>NOT(VLOOKUP(F48,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="11">
+    <cfRule type="expression" dxfId="25" priority="11">
       <formula>(VLOOKUP(F48,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47:H48">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47:H48">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[MS-OXNSPI]: update rs for new NFC bug
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
@@ -11872,6 +11872,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11895,21 +11910,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13388,127 +13388,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -13521,12 +13521,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -13539,12 +13539,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -13557,12 +13557,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -13575,60 +13575,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -51834,8 +51834,8 @@
       <c r="G1524" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H1524" s="22" t="s">
-        <v>20</v>
+      <c r="H1524" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="I1524" s="20" t="s">
         <v>2401</v>
@@ -54676,11 +54676,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -54688,6 +54683,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1542:B1545 A1548:B1549 A1637:I1637 A1634:H1634 D1542:I1545 A1546:I1547 A1550:I1566 D1548:I1549 A1600:I1633 A20:I46 A1570:I1597 E1567:H1569 D1598:H1599 D1635:H1636 G47:G48 I47:K48 A49:I1541">

</xml_diff>

<commit_message>
Updated RS, md and configuration files for MS-OXNSPI(20220215).
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXNSPI/MS-OXNSPI_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D06EAC-73E6-4144-8D84-40377F9565B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B91AC29-F2B6-4AD5-A4CF-C0FB41FAA81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11439,10 +11439,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MS-OXNSPI_R1194001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11459,14 +11455,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MS-OXNSPI_R1194002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does return the value "Success" if SortType field in the input parameter pStat has any value other than SortTypeDisplayName .&lt;6&gt; Section 3.1.4.1.1411:  Exchange 2019 returns "Success".</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In NspiModProps] [Server Processing Rules: Upon receiving message NspiModProps, the server MUST process the data from the message subject to the following constraints:] [Constraint 10] The server SHOULD&lt;7&gt; add all values for all properties specified in the input parameter pRow to the object specified by the field CurrentRec in the input parameter pStat.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11496,10 +11484,6 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] Implementation does return the value "ErrorsReturned" (0x00040380). &lt;5&gt; Section 3.1.4.1.7:  Microsoft Exchange Server 2010 Service Pack 3 (SP3), Exchange 2013, Exchange 2016, and Exchange 2019 return "ErrorsReturned" (0x00040380).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does return the value "GeneralFailure" if SortType field in the input parameter pStat has any value other than SortTypeDisplayName .(Exchange 2007, Exchange 2010, Exchange 2013 and Exchange 2016 follows this behavior)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -11570,7 +11554,19 @@
     <t>[In NspiModLinkAtt] lpEntryIds: A BinaryArray_r value.</t>
   </si>
   <si>
-    <t>13.0</t>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>MS-OXNSPI_R1194002</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does return the value "Success" if SortType field in the input parameter pStat has any value other than SortTypeDisplayName .&lt;6&gt; Section 3.1.4.1.1411:  Exchange 2013, Exchange 2016, and 2019 returns "Success".</t>
+  </si>
+  <si>
+    <t>MS-OXNSPI_R1194001</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does return the value "GeneralFailure" if SortType field in the input parameter pStat has any value other than SortTypeDisplayName .(Exchange 2007, Exchange 2010 follows this behavior)</t>
   </si>
 </sst>
 </file>
@@ -11870,6 +11866,21 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -11893,21 +11904,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13366,8 +13362,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1637"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:I9"/>
+    <sheetView tabSelected="1" topLeftCell="A1517" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1518" sqref="C1518"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -13411,138 +13407,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>3637</v>
+        <v>3633</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>44425</v>
+        <v>44607</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>3634</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
+      <c r="B7" s="39" t="s">
+        <v>3630</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>3635</v>
-      </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="B10" s="47" t="s">
+        <v>3631</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -13555,12 +13551,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -13573,12 +13569,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -13591,12 +13587,12 @@
       <c r="C14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -13609,60 +13605,60 @@
       <c r="C15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -31079,7 +31075,7 @@
         <v>1423</v>
       </c>
       <c r="C705" s="20" t="s">
-        <v>3632</v>
+        <v>3628</v>
       </c>
       <c r="D705" s="22"/>
       <c r="E705" s="22" t="s">
@@ -40870,7 +40866,7 @@
         <v>2264</v>
       </c>
       <c r="C1092" s="20" t="s">
-        <v>3633</v>
+        <v>3629</v>
       </c>
       <c r="D1092" s="22"/>
       <c r="E1092" s="22" t="s">
@@ -41445,7 +41441,7 @@
         <v>2264</v>
       </c>
       <c r="C1115" s="20" t="s">
-        <v>3621</v>
+        <v>3618</v>
       </c>
       <c r="D1115" s="22"/>
       <c r="E1115" s="22" t="s">
@@ -41834,7 +41830,7 @@
         <v>2314</v>
       </c>
       <c r="C1130" s="20" t="s">
-        <v>3636</v>
+        <v>3632</v>
       </c>
       <c r="D1130" s="22"/>
       <c r="E1130" s="22" t="s">
@@ -41961,7 +41957,7 @@
         <v>2314</v>
       </c>
       <c r="C1135" s="20" t="s">
-        <v>3622</v>
+        <v>3619</v>
       </c>
       <c r="D1135" s="22"/>
       <c r="E1135" s="22" t="s">
@@ -51534,7 +51530,7 @@
         <v>3136</v>
       </c>
       <c r="C1512" s="20" t="s">
-        <v>3623</v>
+        <v>3620</v>
       </c>
       <c r="D1512" s="22" t="s">
         <v>3143</v>
@@ -51561,7 +51557,7 @@
         <v>7</v>
       </c>
       <c r="C1513" s="20" t="s">
-        <v>3624</v>
+        <v>3621</v>
       </c>
       <c r="D1513" s="22" t="s">
         <v>3530</v>
@@ -51588,7 +51584,7 @@
         <v>7</v>
       </c>
       <c r="C1514" s="20" t="s">
-        <v>3625</v>
+        <v>3622</v>
       </c>
       <c r="D1514" s="22" t="s">
         <v>3530</v>
@@ -51617,7 +51613,7 @@
         <v>3136</v>
       </c>
       <c r="C1515" s="20" t="s">
-        <v>3626</v>
+        <v>3623</v>
       </c>
       <c r="D1515" s="35" t="s">
         <v>3578</v>
@@ -51644,7 +51640,7 @@
         <v>3136</v>
       </c>
       <c r="C1516" s="20" t="s">
-        <v>3627</v>
+        <v>3624</v>
       </c>
       <c r="D1516" s="35" t="s">
         <v>3579</v>
@@ -51671,7 +51667,7 @@
         <v>7</v>
       </c>
       <c r="C1517" s="20" t="s">
-        <v>3628</v>
+        <v>3625</v>
       </c>
       <c r="D1517" s="22" t="s">
         <v>3531</v>
@@ -51694,16 +51690,16 @@
     </row>
     <row r="1518" spans="1:9" ht="45">
       <c r="A1518" s="22" t="s">
+        <v>3636</v>
+      </c>
+      <c r="B1518" s="25" t="s">
         <v>3614</v>
       </c>
-      <c r="B1518" s="25" t="s">
-        <v>3615</v>
-      </c>
       <c r="C1518" s="20" t="s">
-        <v>3629</v>
+        <v>3637</v>
       </c>
       <c r="D1518" s="22" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="E1518" s="22" t="s">
         <v>22</v>
@@ -51723,16 +51719,16 @@
     </row>
     <row r="1519" spans="1:9" ht="45">
       <c r="A1519" s="22" t="s">
-        <v>3619</v>
+        <v>3634</v>
       </c>
       <c r="B1519" s="25" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="C1519" s="20" t="s">
-        <v>3620</v>
+        <v>3635</v>
       </c>
       <c r="D1519" s="22" t="s">
-        <v>3618</v>
+        <v>3617</v>
       </c>
       <c r="E1519" s="22" t="s">
         <v>22</v>
@@ -51758,10 +51754,10 @@
         <v>7</v>
       </c>
       <c r="C1520" s="20" t="s">
-        <v>3630</v>
+        <v>3626</v>
       </c>
       <c r="D1520" s="22" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="E1520" s="30" t="s">
         <v>22</v>
@@ -51785,7 +51781,7 @@
         <v>7</v>
       </c>
       <c r="C1521" s="20" t="s">
-        <v>3631</v>
+        <v>3627</v>
       </c>
       <c r="D1521" s="22" t="s">
         <v>3532</v>
@@ -51814,7 +51810,7 @@
         <v>7</v>
       </c>
       <c r="C1522" s="20" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="D1522" s="22" t="s">
         <v>3532</v>
@@ -54612,11 +54608,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -54624,6 +54615,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1538:B1541 A1544:B1545 A1633:I1633 A1630:H1630 D1538:I1541 A1542:I1543 A1546:I1562 D1544:I1545 A1596:I1629 A20:I46 A1566:I1593 E1563:H1565 D1594:H1595 D1631:H1632 G47:G48 I47:K48 A49:I1537">

</xml_diff>